<commit_message>
working on emissions zonal stats but didn't finish the code
</commit_message>
<xml_diff>
--- a/outputs/y2y_carbon_biomes.xlsx
+++ b/outputs/y2y_carbon_biomes.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bermane/Team Braintree Dropbox/Ethan Berman/Python Projects/y2y-carbon/outputs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49FD0A83-6056-B445-9643-E21747BD5522}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FCFB35D-1704-AA4B-B836-D23BEB2F1C46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10660" yWindow="500" windowWidth="42680" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="32000" yWindow="500" windowWidth="32000" windowHeight="26160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>